<commit_message>
feat: Updated excel files of analytic data
</commit_message>
<xml_diff>
--- a/tabular/training-validation-data.xlsx
+++ b/tabular/training-validation-data.xlsx
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5260416865348816</v>
+        <v>0.70703125</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6260775923728943</v>
+        <v>0.6849056482315063</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5729166865348816</v>
+        <v>0.88671875</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7322198152542114</v>
+        <v>0.9448113441467285</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5208333134651184</v>
+        <v>0.91015625</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8933189511299133</v>
+        <v>0.9886792302131653</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.59375</v>
+        <v>0.91796875</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9445043206214905</v>
+        <v>0.9990565776824951</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +514,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6197916865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9784482717514038</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5729166865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9401939511299133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -542,10 +542,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6197916865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D8" t="n">
-        <v>0.982758641242981</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -556,10 +556,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5729166865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9795258641242981</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5885416865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9956896305084229</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -584,10 +584,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6197916865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9730603694915771</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -598,10 +598,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6041666865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9962284564971924</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.91796875</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -626,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5885416865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -640,7 +640,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6041666865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -654,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5885416865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -668,7 +668,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5885416865348816</v>
+        <v>0.91796875</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -682,7 +682,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.91796875</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -696,7 +696,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.91796875</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.91796875</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -724,7 +724,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.91796875</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.9140625</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.9140625</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.9140625</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -780,7 +780,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.9140625</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5989583134651184</v>
+        <v>0.921875</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>

</xml_diff>